<commit_message>
Updated line text for the ChangingLines component.
</commit_message>
<xml_diff>
--- a/Daily Activits.xlsx
+++ b/Daily Activits.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="362">
   <si>
     <t>DATE</t>
   </si>
@@ -940,21 +940,12 @@
     <t>Added component to show associated hexagrams.</t>
   </si>
   <si>
-    <t>Febuary 3 2018</t>
-  </si>
-  <si>
     <t>Meeting with Spring to get new requirements and put them in the Github.</t>
   </si>
   <si>
-    <t>Febuary 4 2018</t>
-  </si>
-  <si>
     <t>Resolved #16</t>
   </si>
   <si>
-    <t>Febuary 5 2018</t>
-  </si>
-  <si>
     <t>Finised HexagramListContainer component.</t>
   </si>
   <si>
@@ -964,9 +955,6 @@
     <t>Fixed two bugs. Added test code for HexagramListContainer component.</t>
   </si>
   <si>
-    <t>Febuary 6 2018</t>
-  </si>
-  <si>
     <t>Added BigramSmallClock component as well as test code.</t>
   </si>
   <si>
@@ -976,15 +964,9 @@
     <t>Working on hexagram detail page.</t>
   </si>
   <si>
-    <t>Febuary 7 2018</t>
-  </si>
-  <si>
     <t>Finished hexagram detail page.</t>
   </si>
   <si>
-    <t>Febuary 9 2018</t>
-  </si>
-  <si>
     <t>Finished BigramClockBig component.</t>
   </si>
   <si>
@@ -994,15 +976,9 @@
     <t>Started making BigramBlockBig component.</t>
   </si>
   <si>
-    <t>Febuary 10 2018</t>
-  </si>
-  <si>
     <t xml:space="preserve">Connected HexagramDetailModal with ReadingsContainer component. </t>
   </si>
   <si>
-    <t>Febuary 11 2018</t>
-  </si>
-  <si>
     <t>Refinement of the Hexagram Page.</t>
   </si>
   <si>
@@ -1012,18 +988,12 @@
     <t>Changed Navbar and started to add quartet bigrams to hexagram database.</t>
   </si>
   <si>
-    <t>Febuary 12 2018</t>
-  </si>
-  <si>
     <t>Adjust hexagram detail display page.</t>
   </si>
   <si>
     <t>Working on add Resonance Quartet Hexagrams.</t>
   </si>
   <si>
-    <t>Febuary 13 2018</t>
-  </si>
-  <si>
     <t>Finished adding resonance quartet hexagrams.</t>
   </si>
   <si>
@@ -1033,45 +1003,24 @@
     <t>Working on add line changing to hexagram.</t>
   </si>
   <si>
-    <t>Febuary 14 2018</t>
-  </si>
-  <si>
     <t>Finished add line changing.</t>
   </si>
   <si>
-    <t>Febuary 15 2018</t>
-  </si>
-  <si>
     <t>Changed some display text.</t>
   </si>
   <si>
-    <t>Febuary 16 2018</t>
-  </si>
-  <si>
     <t>Working on automatically update Resonance code name in HexagramDetailModal componnet.</t>
   </si>
   <si>
     <t>Finished automatically update Resonance code name in HexagramDetailModal componnet.</t>
   </si>
   <si>
-    <t>Febuary 17 2018</t>
-  </si>
-  <si>
-    <t>Febuary 18 2018</t>
-  </si>
-  <si>
-    <t>Febuary 19 2018</t>
-  </si>
-  <si>
     <t>Fixed some bugs that include hexagram detail modal display incorrectly on the small mobile screen, etc.</t>
   </si>
   <si>
     <t xml:space="preserve">Trying to implement code splitting with react-loadable labaary </t>
   </si>
   <si>
-    <t>Febuary 20 2018</t>
-  </si>
-  <si>
     <t>Researching customizing name for the chunk bundles.</t>
   </si>
   <si>
@@ -1094,6 +1043,75 @@
   </si>
   <si>
     <t>Improving the performance. Switched to http2</t>
+  </si>
+  <si>
+    <t>February 20 2018</t>
+  </si>
+  <si>
+    <t>February 19 2018</t>
+  </si>
+  <si>
+    <t>February 18 2018</t>
+  </si>
+  <si>
+    <t>February 17 2018</t>
+  </si>
+  <si>
+    <t>February 16 2018</t>
+  </si>
+  <si>
+    <t>February 15 2018</t>
+  </si>
+  <si>
+    <t>February 14 2018</t>
+  </si>
+  <si>
+    <t>February 13 2018</t>
+  </si>
+  <si>
+    <t>February 12 2018</t>
+  </si>
+  <si>
+    <t>February 11 2018</t>
+  </si>
+  <si>
+    <t>February 10 2018</t>
+  </si>
+  <si>
+    <t>February 9 2018</t>
+  </si>
+  <si>
+    <t>February 7 2018</t>
+  </si>
+  <si>
+    <t>February 6 2018</t>
+  </si>
+  <si>
+    <t>February 5 2018</t>
+  </si>
+  <si>
+    <t>February 4 2018</t>
+  </si>
+  <si>
+    <t>February 3 2018</t>
+  </si>
+  <si>
+    <t>February 22 2018</t>
+  </si>
+  <si>
+    <t>Changed add journal button's color. Added showing hexagram detail modal feature to search reading page.</t>
+  </si>
+  <si>
+    <t>February 23 2018</t>
+  </si>
+  <si>
+    <t>Starting to extract some code relates to show hexagram detail modal.</t>
+  </si>
+  <si>
+    <t>Finished refactoring for HexagramDetailModal.</t>
+  </si>
+  <si>
+    <t>February 24 2018</t>
   </si>
 </sst>
 </file>
@@ -11873,8 +11891,8 @@
   </sheetPr>
   <dimension ref="B1:F328"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A311" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F310" sqref="F310"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A305" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C320" sqref="C320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -12086,7 +12104,7 @@
         <v>0.10763888888888895</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16493,7 +16511,7 @@
     </row>
     <row r="275" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B275" s="3" t="s">
-        <v>304</v>
+        <v>355</v>
       </c>
       <c r="C275" s="2">
         <v>0.54166666666666663</v>
@@ -16506,12 +16524,12 @@
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="F275" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="276" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B276" s="3" t="s">
-        <v>306</v>
+        <v>354</v>
       </c>
       <c r="C276" s="2">
         <v>0.44444444444444442</v>
@@ -16524,7 +16542,7 @@
         <v>9.722222222222221E-2</v>
       </c>
       <c r="F276" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="277" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16540,12 +16558,12 @@
         <v>4.2361111111111183E-2</v>
       </c>
       <c r="F277" s="8" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="278" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B278" s="3" t="s">
-        <v>308</v>
+        <v>353</v>
       </c>
       <c r="C278" s="2">
         <v>0.70833333333333337</v>
@@ -16558,7 +16576,7 @@
         <v>4.861111111111116E-2</v>
       </c>
       <c r="F278" s="8" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="279" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16574,12 +16592,12 @@
         <v>6.8055555555555536E-2</v>
       </c>
       <c r="F279" s="8" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="280" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B280" s="3" t="s">
-        <v>312</v>
+        <v>352</v>
       </c>
       <c r="C280" s="2">
         <v>0.45069444444444445</v>
@@ -16592,7 +16610,7 @@
         <v>7.0833333333333359E-2</v>
       </c>
       <c r="F280" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="281" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16608,7 +16626,7 @@
         <v>0.1694444444444444</v>
       </c>
       <c r="F281" s="8" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="282" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16624,12 +16642,12 @@
         <v>7.1527777777777857E-2</v>
       </c>
       <c r="F282" s="8" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="283" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B283" s="3" t="s">
-        <v>316</v>
+        <v>351</v>
       </c>
       <c r="C283" s="2">
         <v>0.45833333333333331</v>
@@ -16642,7 +16660,7 @@
         <v>1.0416666666666685E-2</v>
       </c>
       <c r="F283" s="8" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="284" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16658,12 +16676,12 @@
         <v>8.4027777777777812E-2</v>
       </c>
       <c r="F284" s="8" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="285" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B285" s="3" t="s">
-        <v>318</v>
+        <v>350</v>
       </c>
       <c r="C285" s="2">
         <v>0.6166666666666667</v>
@@ -16676,7 +16694,7 @@
         <v>8.4027777777777701E-2</v>
       </c>
       <c r="F285" s="8" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="286" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16692,7 +16710,7 @@
         <v>9.7222222222222987E-3</v>
       </c>
       <c r="F286" s="8" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="287" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16708,12 +16726,12 @@
         <v>9.375E-2</v>
       </c>
       <c r="F287" s="8" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="288" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B288" s="3" t="s">
-        <v>322</v>
+        <v>349</v>
       </c>
       <c r="C288" s="2">
         <v>0.37708333333333338</v>
@@ -16726,7 +16744,7 @@
         <v>1.8749999999999933E-2</v>
       </c>
       <c r="F288" s="8" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="289" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16742,7 +16760,7 @@
         <v>2.083333333333337E-2</v>
       </c>
       <c r="F289" s="8" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="290" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16758,7 +16776,7 @@
         <v>2.5694444444444464E-2</v>
       </c>
       <c r="F290" s="8" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="291" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16774,12 +16792,12 @@
         <v>7.4305555555555403E-2</v>
       </c>
       <c r="F291" s="8" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
     </row>
     <row r="292" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B292" s="3" t="s">
-        <v>324</v>
+        <v>348</v>
       </c>
       <c r="C292" s="2">
         <v>0.51388888888888895</v>
@@ -16792,7 +16810,7 @@
         <v>3.4722222222222099E-2</v>
       </c>
       <c r="F292" s="8" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
     </row>
     <row r="293" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16808,7 +16826,7 @@
         <v>5.4166666666666696E-2</v>
       </c>
       <c r="F293" s="8" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="294" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16824,12 +16842,12 @@
         <v>5.9722222222222232E-2</v>
       </c>
       <c r="F294" s="8" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
     </row>
     <row r="295" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B295" s="3" t="s">
-        <v>328</v>
+        <v>347</v>
       </c>
       <c r="C295" s="2">
         <v>0.6875</v>
@@ -16842,7 +16860,7 @@
         <v>7.7777777777777835E-2</v>
       </c>
       <c r="F295" s="8" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="296" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16858,12 +16876,12 @@
         <v>6.1111111111111227E-2</v>
       </c>
       <c r="F296" s="8" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="297" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B297" s="3" t="s">
-        <v>331</v>
+        <v>346</v>
       </c>
       <c r="C297" s="2">
         <v>0.43402777777777773</v>
@@ -16876,7 +16894,7 @@
         <v>5.4166666666666696E-2</v>
       </c>
       <c r="F297" s="8" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="298" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16892,7 +16910,7 @@
         <v>1.0416666666666741E-2</v>
       </c>
       <c r="F298" s="8" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="299" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16908,7 +16926,7 @@
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="F299" s="8" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="300" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16924,12 +16942,12 @@
         <v>6.8055555555555536E-2</v>
       </c>
       <c r="F300" s="8" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="301" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B301" s="3" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="C301" s="2">
         <v>0.45208333333333334</v>
@@ -16942,12 +16960,12 @@
         <v>9.930555555555548E-2</v>
       </c>
       <c r="F301" s="8" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="302" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B302" s="3" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="C302" s="2">
         <v>0.24444444444444446</v>
@@ -16960,12 +16978,12 @@
         <v>1.9444444444444431E-2</v>
       </c>
       <c r="F302" s="8" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
     </row>
     <row r="303" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B303" s="3" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C303" s="2">
         <v>0.48749999999999999</v>
@@ -16978,7 +16996,7 @@
         <v>3.3333333333333381E-2</v>
       </c>
       <c r="F303" s="8" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
     </row>
     <row r="304" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16994,7 +17012,7 @@
         <v>4.166666666666663E-2</v>
       </c>
       <c r="F304" s="8" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
     </row>
     <row r="305" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17012,7 +17030,7 @@
         <v>4.9305555555555602E-2</v>
       </c>
       <c r="F305" s="8" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
     </row>
     <row r="306" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17028,7 +17046,7 @@
         <v>0.11805555555555558</v>
       </c>
       <c r="F306" s="8" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
     </row>
     <row r="307" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17044,12 +17062,12 @@
         <v>0.10416666666666663</v>
       </c>
       <c r="F307" s="8" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
     </row>
     <row r="308" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B308" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C308" s="2">
         <v>0.45833333333333331</v>
@@ -17062,7 +17080,7 @@
         <v>6.9444444444444475E-2</v>
       </c>
       <c r="F308" s="8" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
     </row>
     <row r="309" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17078,7 +17096,7 @@
         <v>0.15277777777777768</v>
       </c>
       <c r="F309" s="8" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
     </row>
     <row r="310" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17094,12 +17112,12 @@
         <v>7.5000000000000067E-2</v>
       </c>
       <c r="F310" s="8" t="s">
-        <v>355</v>
+        <v>338</v>
       </c>
     </row>
     <row r="311" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B311" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C311" s="2">
         <v>0.5756944444444444</v>
@@ -17112,7 +17130,7 @@
         <v>0.17291666666666661</v>
       </c>
       <c r="F311" s="8" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
     </row>
     <row r="312" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17128,12 +17146,12 @@
         <v>0.14097222222222217</v>
       </c>
       <c r="F312" s="8" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
     </row>
     <row r="313" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B313" s="3" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="C313" s="2">
         <v>0</v>
@@ -17146,7 +17164,7 @@
         <v>4.9305555555555554E-2</v>
       </c>
       <c r="F313" s="8" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
     </row>
     <row r="314" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17162,7 +17180,7 @@
         <v>6.9444444444444475E-2</v>
       </c>
       <c r="F314" s="8" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
     </row>
     <row r="315" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17178,7 +17196,7 @@
         <v>0.10763888888888895</v>
       </c>
       <c r="F315" s="8" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
     </row>
     <row r="316" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17194,46 +17212,72 @@
         <v>0.12361111111111101</v>
       </c>
       <c r="F316" s="8" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
     </row>
     <row r="317" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B317" s="3"/>
-      <c r="C317" s="2"/>
-      <c r="D317" s="2"/>
+      <c r="B317" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C317" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D317" s="2">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="E317" s="10">
         <f>Log[[#This Row],[EDN TIME]]-Log[[#This Row],[START TIME]]</f>
-        <v>0</v>
-      </c>
-      <c r="F317" s="4"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F317" s="8" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="318" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B318" s="3"/>
-      <c r="C318" s="2"/>
-      <c r="D318" s="2"/>
+      <c r="B318" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C318" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D318" s="2">
+        <v>0.75</v>
+      </c>
       <c r="E318" s="10">
         <f>Log[[#This Row],[EDN TIME]]-Log[[#This Row],[START TIME]]</f>
-        <v>0</v>
-      </c>
-      <c r="F318" s="4"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F318" s="8" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="319" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B319" s="3"/>
-      <c r="C319" s="2"/>
-      <c r="D319" s="2"/>
+      <c r="C319" s="2">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="D319" s="2">
+        <v>1.0326388888888889</v>
+      </c>
       <c r="E319" s="10">
         <f>Log[[#This Row],[EDN TIME]]-Log[[#This Row],[START TIME]]</f>
-        <v>0</v>
-      </c>
-      <c r="F319" s="4"/>
+        <v>0.17152777777777772</v>
+      </c>
+      <c r="F319" s="8" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="320" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B320" s="3"/>
-      <c r="C320" s="2"/>
+      <c r="B320" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C320" s="2">
+        <v>0.65763888888888888</v>
+      </c>
       <c r="D320" s="2"/>
       <c r="E320" s="10">
         <f>Log[[#This Row],[EDN TIME]]-Log[[#This Row],[START TIME]]</f>
-        <v>0</v>
+        <v>-0.65763888888888888</v>
       </c>
       <c r="F320" s="4"/>
     </row>

</xml_diff>

<commit_message>
Updated line text for the ChangingLines component. (#94)
</commit_message>
<xml_diff>
--- a/Daily Activits.xlsx
+++ b/Daily Activits.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="362">
   <si>
     <t>DATE</t>
   </si>
@@ -940,21 +940,12 @@
     <t>Added component to show associated hexagrams.</t>
   </si>
   <si>
-    <t>Febuary 3 2018</t>
-  </si>
-  <si>
     <t>Meeting with Spring to get new requirements and put them in the Github.</t>
   </si>
   <si>
-    <t>Febuary 4 2018</t>
-  </si>
-  <si>
     <t>Resolved #16</t>
   </si>
   <si>
-    <t>Febuary 5 2018</t>
-  </si>
-  <si>
     <t>Finised HexagramListContainer component.</t>
   </si>
   <si>
@@ -964,9 +955,6 @@
     <t>Fixed two bugs. Added test code for HexagramListContainer component.</t>
   </si>
   <si>
-    <t>Febuary 6 2018</t>
-  </si>
-  <si>
     <t>Added BigramSmallClock component as well as test code.</t>
   </si>
   <si>
@@ -976,15 +964,9 @@
     <t>Working on hexagram detail page.</t>
   </si>
   <si>
-    <t>Febuary 7 2018</t>
-  </si>
-  <si>
     <t>Finished hexagram detail page.</t>
   </si>
   <si>
-    <t>Febuary 9 2018</t>
-  </si>
-  <si>
     <t>Finished BigramClockBig component.</t>
   </si>
   <si>
@@ -994,15 +976,9 @@
     <t>Started making BigramBlockBig component.</t>
   </si>
   <si>
-    <t>Febuary 10 2018</t>
-  </si>
-  <si>
     <t xml:space="preserve">Connected HexagramDetailModal with ReadingsContainer component. </t>
   </si>
   <si>
-    <t>Febuary 11 2018</t>
-  </si>
-  <si>
     <t>Refinement of the Hexagram Page.</t>
   </si>
   <si>
@@ -1012,18 +988,12 @@
     <t>Changed Navbar and started to add quartet bigrams to hexagram database.</t>
   </si>
   <si>
-    <t>Febuary 12 2018</t>
-  </si>
-  <si>
     <t>Adjust hexagram detail display page.</t>
   </si>
   <si>
     <t>Working on add Resonance Quartet Hexagrams.</t>
   </si>
   <si>
-    <t>Febuary 13 2018</t>
-  </si>
-  <si>
     <t>Finished adding resonance quartet hexagrams.</t>
   </si>
   <si>
@@ -1033,45 +1003,24 @@
     <t>Working on add line changing to hexagram.</t>
   </si>
   <si>
-    <t>Febuary 14 2018</t>
-  </si>
-  <si>
     <t>Finished add line changing.</t>
   </si>
   <si>
-    <t>Febuary 15 2018</t>
-  </si>
-  <si>
     <t>Changed some display text.</t>
   </si>
   <si>
-    <t>Febuary 16 2018</t>
-  </si>
-  <si>
     <t>Working on automatically update Resonance code name in HexagramDetailModal componnet.</t>
   </si>
   <si>
     <t>Finished automatically update Resonance code name in HexagramDetailModal componnet.</t>
   </si>
   <si>
-    <t>Febuary 17 2018</t>
-  </si>
-  <si>
-    <t>Febuary 18 2018</t>
-  </si>
-  <si>
-    <t>Febuary 19 2018</t>
-  </si>
-  <si>
     <t>Fixed some bugs that include hexagram detail modal display incorrectly on the small mobile screen, etc.</t>
   </si>
   <si>
     <t xml:space="preserve">Trying to implement code splitting with react-loadable labaary </t>
   </si>
   <si>
-    <t>Febuary 20 2018</t>
-  </si>
-  <si>
     <t>Researching customizing name for the chunk bundles.</t>
   </si>
   <si>
@@ -1094,6 +1043,75 @@
   </si>
   <si>
     <t>Improving the performance. Switched to http2</t>
+  </si>
+  <si>
+    <t>February 20 2018</t>
+  </si>
+  <si>
+    <t>February 19 2018</t>
+  </si>
+  <si>
+    <t>February 18 2018</t>
+  </si>
+  <si>
+    <t>February 17 2018</t>
+  </si>
+  <si>
+    <t>February 16 2018</t>
+  </si>
+  <si>
+    <t>February 15 2018</t>
+  </si>
+  <si>
+    <t>February 14 2018</t>
+  </si>
+  <si>
+    <t>February 13 2018</t>
+  </si>
+  <si>
+    <t>February 12 2018</t>
+  </si>
+  <si>
+    <t>February 11 2018</t>
+  </si>
+  <si>
+    <t>February 10 2018</t>
+  </si>
+  <si>
+    <t>February 9 2018</t>
+  </si>
+  <si>
+    <t>February 7 2018</t>
+  </si>
+  <si>
+    <t>February 6 2018</t>
+  </si>
+  <si>
+    <t>February 5 2018</t>
+  </si>
+  <si>
+    <t>February 4 2018</t>
+  </si>
+  <si>
+    <t>February 3 2018</t>
+  </si>
+  <si>
+    <t>February 22 2018</t>
+  </si>
+  <si>
+    <t>Changed add journal button's color. Added showing hexagram detail modal feature to search reading page.</t>
+  </si>
+  <si>
+    <t>February 23 2018</t>
+  </si>
+  <si>
+    <t>Starting to extract some code relates to show hexagram detail modal.</t>
+  </si>
+  <si>
+    <t>Finished refactoring for HexagramDetailModal.</t>
+  </si>
+  <si>
+    <t>February 24 2018</t>
   </si>
 </sst>
 </file>
@@ -11873,8 +11891,8 @@
   </sheetPr>
   <dimension ref="B1:F328"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A311" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F310" sqref="F310"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A305" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C320" sqref="C320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -12086,7 +12104,7 @@
         <v>0.10763888888888895</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16493,7 +16511,7 @@
     </row>
     <row r="275" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B275" s="3" t="s">
-        <v>304</v>
+        <v>355</v>
       </c>
       <c r="C275" s="2">
         <v>0.54166666666666663</v>
@@ -16506,12 +16524,12 @@
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="F275" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="276" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B276" s="3" t="s">
-        <v>306</v>
+        <v>354</v>
       </c>
       <c r="C276" s="2">
         <v>0.44444444444444442</v>
@@ -16524,7 +16542,7 @@
         <v>9.722222222222221E-2</v>
       </c>
       <c r="F276" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="277" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16540,12 +16558,12 @@
         <v>4.2361111111111183E-2</v>
       </c>
       <c r="F277" s="8" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="278" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B278" s="3" t="s">
-        <v>308</v>
+        <v>353</v>
       </c>
       <c r="C278" s="2">
         <v>0.70833333333333337</v>
@@ -16558,7 +16576,7 @@
         <v>4.861111111111116E-2</v>
       </c>
       <c r="F278" s="8" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="279" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16574,12 +16592,12 @@
         <v>6.8055555555555536E-2</v>
       </c>
       <c r="F279" s="8" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="280" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B280" s="3" t="s">
-        <v>312</v>
+        <v>352</v>
       </c>
       <c r="C280" s="2">
         <v>0.45069444444444445</v>
@@ -16592,7 +16610,7 @@
         <v>7.0833333333333359E-2</v>
       </c>
       <c r="F280" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="281" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16608,7 +16626,7 @@
         <v>0.1694444444444444</v>
       </c>
       <c r="F281" s="8" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="282" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16624,12 +16642,12 @@
         <v>7.1527777777777857E-2</v>
       </c>
       <c r="F282" s="8" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="283" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B283" s="3" t="s">
-        <v>316</v>
+        <v>351</v>
       </c>
       <c r="C283" s="2">
         <v>0.45833333333333331</v>
@@ -16642,7 +16660,7 @@
         <v>1.0416666666666685E-2</v>
       </c>
       <c r="F283" s="8" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="284" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16658,12 +16676,12 @@
         <v>8.4027777777777812E-2</v>
       </c>
       <c r="F284" s="8" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="285" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B285" s="3" t="s">
-        <v>318</v>
+        <v>350</v>
       </c>
       <c r="C285" s="2">
         <v>0.6166666666666667</v>
@@ -16676,7 +16694,7 @@
         <v>8.4027777777777701E-2</v>
       </c>
       <c r="F285" s="8" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="286" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16692,7 +16710,7 @@
         <v>9.7222222222222987E-3</v>
       </c>
       <c r="F286" s="8" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="287" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16708,12 +16726,12 @@
         <v>9.375E-2</v>
       </c>
       <c r="F287" s="8" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="288" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B288" s="3" t="s">
-        <v>322</v>
+        <v>349</v>
       </c>
       <c r="C288" s="2">
         <v>0.37708333333333338</v>
@@ -16726,7 +16744,7 @@
         <v>1.8749999999999933E-2</v>
       </c>
       <c r="F288" s="8" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="289" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16742,7 +16760,7 @@
         <v>2.083333333333337E-2</v>
       </c>
       <c r="F289" s="8" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="290" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16758,7 +16776,7 @@
         <v>2.5694444444444464E-2</v>
       </c>
       <c r="F290" s="8" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="291" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16774,12 +16792,12 @@
         <v>7.4305555555555403E-2</v>
       </c>
       <c r="F291" s="8" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
     </row>
     <row r="292" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B292" s="3" t="s">
-        <v>324</v>
+        <v>348</v>
       </c>
       <c r="C292" s="2">
         <v>0.51388888888888895</v>
@@ -16792,7 +16810,7 @@
         <v>3.4722222222222099E-2</v>
       </c>
       <c r="F292" s="8" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
     </row>
     <row r="293" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16808,7 +16826,7 @@
         <v>5.4166666666666696E-2</v>
       </c>
       <c r="F293" s="8" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="294" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16824,12 +16842,12 @@
         <v>5.9722222222222232E-2</v>
       </c>
       <c r="F294" s="8" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
     </row>
     <row r="295" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B295" s="3" t="s">
-        <v>328</v>
+        <v>347</v>
       </c>
       <c r="C295" s="2">
         <v>0.6875</v>
@@ -16842,7 +16860,7 @@
         <v>7.7777777777777835E-2</v>
       </c>
       <c r="F295" s="8" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="296" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16858,12 +16876,12 @@
         <v>6.1111111111111227E-2</v>
       </c>
       <c r="F296" s="8" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="297" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B297" s="3" t="s">
-        <v>331</v>
+        <v>346</v>
       </c>
       <c r="C297" s="2">
         <v>0.43402777777777773</v>
@@ -16876,7 +16894,7 @@
         <v>5.4166666666666696E-2</v>
       </c>
       <c r="F297" s="8" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="298" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16892,7 +16910,7 @@
         <v>1.0416666666666741E-2</v>
       </c>
       <c r="F298" s="8" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="299" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16908,7 +16926,7 @@
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="F299" s="8" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="300" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16924,12 +16942,12 @@
         <v>6.8055555555555536E-2</v>
       </c>
       <c r="F300" s="8" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="301" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B301" s="3" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="C301" s="2">
         <v>0.45208333333333334</v>
@@ -16942,12 +16960,12 @@
         <v>9.930555555555548E-2</v>
       </c>
       <c r="F301" s="8" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="302" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B302" s="3" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="C302" s="2">
         <v>0.24444444444444446</v>
@@ -16960,12 +16978,12 @@
         <v>1.9444444444444431E-2</v>
       </c>
       <c r="F302" s="8" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
     </row>
     <row r="303" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B303" s="3" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C303" s="2">
         <v>0.48749999999999999</v>
@@ -16978,7 +16996,7 @@
         <v>3.3333333333333381E-2</v>
       </c>
       <c r="F303" s="8" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
     </row>
     <row r="304" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16994,7 +17012,7 @@
         <v>4.166666666666663E-2</v>
       </c>
       <c r="F304" s="8" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
     </row>
     <row r="305" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17012,7 +17030,7 @@
         <v>4.9305555555555602E-2</v>
       </c>
       <c r="F305" s="8" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
     </row>
     <row r="306" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17028,7 +17046,7 @@
         <v>0.11805555555555558</v>
       </c>
       <c r="F306" s="8" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
     </row>
     <row r="307" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17044,12 +17062,12 @@
         <v>0.10416666666666663</v>
       </c>
       <c r="F307" s="8" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
     </row>
     <row r="308" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B308" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C308" s="2">
         <v>0.45833333333333331</v>
@@ -17062,7 +17080,7 @@
         <v>6.9444444444444475E-2</v>
       </c>
       <c r="F308" s="8" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
     </row>
     <row r="309" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17078,7 +17096,7 @@
         <v>0.15277777777777768</v>
       </c>
       <c r="F309" s="8" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
     </row>
     <row r="310" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17094,12 +17112,12 @@
         <v>7.5000000000000067E-2</v>
       </c>
       <c r="F310" s="8" t="s">
-        <v>355</v>
+        <v>338</v>
       </c>
     </row>
     <row r="311" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B311" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C311" s="2">
         <v>0.5756944444444444</v>
@@ -17112,7 +17130,7 @@
         <v>0.17291666666666661</v>
       </c>
       <c r="F311" s="8" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
     </row>
     <row r="312" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17128,12 +17146,12 @@
         <v>0.14097222222222217</v>
       </c>
       <c r="F312" s="8" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
     </row>
     <row r="313" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B313" s="3" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="C313" s="2">
         <v>0</v>
@@ -17146,7 +17164,7 @@
         <v>4.9305555555555554E-2</v>
       </c>
       <c r="F313" s="8" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
     </row>
     <row r="314" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17162,7 +17180,7 @@
         <v>6.9444444444444475E-2</v>
       </c>
       <c r="F314" s="8" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
     </row>
     <row r="315" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17178,7 +17196,7 @@
         <v>0.10763888888888895</v>
       </c>
       <c r="F315" s="8" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
     </row>
     <row r="316" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17194,46 +17212,72 @@
         <v>0.12361111111111101</v>
       </c>
       <c r="F316" s="8" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
     </row>
     <row r="317" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B317" s="3"/>
-      <c r="C317" s="2"/>
-      <c r="D317" s="2"/>
+      <c r="B317" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C317" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D317" s="2">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="E317" s="10">
         <f>Log[[#This Row],[EDN TIME]]-Log[[#This Row],[START TIME]]</f>
-        <v>0</v>
-      </c>
-      <c r="F317" s="4"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F317" s="8" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="318" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B318" s="3"/>
-      <c r="C318" s="2"/>
-      <c r="D318" s="2"/>
+      <c r="B318" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C318" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D318" s="2">
+        <v>0.75</v>
+      </c>
       <c r="E318" s="10">
         <f>Log[[#This Row],[EDN TIME]]-Log[[#This Row],[START TIME]]</f>
-        <v>0</v>
-      </c>
-      <c r="F318" s="4"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F318" s="8" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="319" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B319" s="3"/>
-      <c r="C319" s="2"/>
-      <c r="D319" s="2"/>
+      <c r="C319" s="2">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="D319" s="2">
+        <v>1.0326388888888889</v>
+      </c>
       <c r="E319" s="10">
         <f>Log[[#This Row],[EDN TIME]]-Log[[#This Row],[START TIME]]</f>
-        <v>0</v>
-      </c>
-      <c r="F319" s="4"/>
+        <v>0.17152777777777772</v>
+      </c>
+      <c r="F319" s="8" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="320" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B320" s="3"/>
-      <c r="C320" s="2"/>
+      <c r="B320" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C320" s="2">
+        <v>0.65763888888888888</v>
+      </c>
       <c r="D320" s="2"/>
       <c r="E320" s="10">
         <f>Log[[#This Row],[EDN TIME]]-Log[[#This Row],[START TIME]]</f>
-        <v>0</v>
+        <v>-0.65763888888888888</v>
       </c>
       <c r="F320" s="4"/>
     </row>

</xml_diff>